<commit_message>
trying to get text parsing done for an easier way to script the chapters
</commit_message>
<xml_diff>
--- a/Assets/Text/Chapter1.xlsx
+++ b/Assets/Text/Chapter1.xlsx
@@ -34,7 +34,7 @@
     <t>End</t>
   </si>
   <si>
-    <t/>
+    <t>asf</t>
   </si>
 </sst>
 </file>
@@ -84,15 +84,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -400,7 +403,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -408,7 +411,7 @@
   <cols>
     <col min="1" max="1" style="4" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="4" width="87.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="44.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="44.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -429,16 +432,26 @@
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C5" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>